<commit_message>
renforcement modele bdd, ajout fichier excel type defaut.
</commit_message>
<xml_diff>
--- a/SonarLysaFX/src/test/resources/Plantage.xlsx
+++ b/SonarLysaFX/src/test/resources/Plantage.xlsx
@@ -11,11 +11,11 @@
     <sheet name="E31" sheetId="68" r:id="rId2"/>
     <sheet name="E30" sheetId="69" r:id="rId3"/>
     <sheet name="E32" sheetId="70" r:id="rId4"/>
-    <sheet name="SUIVI Qualité" sheetId="71" r:id="rId5"/>
+    <sheet name="SUIVI Défaults Qualité" sheetId="71" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Anomalies closes'!$A$1:$V$34</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'SUIVI Qualité'!$E$1:$E$22</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'SUIVI Défaults Qualité'!$E$1:$E$22</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -7712,7 +7712,7 @@
   <dimension ref="A1:T22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>